<commit_message>
replaced empty values with zeroes in Dataset v2
</commit_message>
<xml_diff>
--- a/Dataset_modified.xlsx
+++ b/Dataset_modified.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="35">
   <si>
     <t>01BPLJ20</t>
   </si>
@@ -235,9 +235,6 @@
       </rPr>
       <t>%</t>
     </r>
-  </si>
-  <si>
-    <t>NaN</t>
   </si>
 </sst>
 </file>
@@ -12313,8 +12310,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13213,12 +13210,8 @@
       <c r="M21" s="1">
         <v>6.2</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -14179,9 +14172,7 @@
       <c r="F42" s="1">
         <v>9.6999999999999993</v>
       </c>
-      <c r="G42" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="G42" s="1"/>
       <c r="H42" s="1">
         <v>21.7</v>
       </c>
@@ -14203,9 +14194,7 @@
       <c r="N42" s="1">
         <v>0.7</v>
       </c>
-      <c r="O42" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="O42" s="1"/>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">

</xml_diff>

<commit_message>
added MultinomialNB algorithm, changed sheet name from rel.vlažnost to rel.vlaznost
</commit_message>
<xml_diff>
--- a/Dataset_modified.xlsx
+++ b/Dataset_modified.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15180" windowHeight="8070" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15180" windowHeight="8070"/>
   </bookViews>
   <sheets>
-    <sheet name="rel.vlažnost" sheetId="1" r:id="rId1"/>
+    <sheet name="rel.vlaznost" sheetId="1" r:id="rId1"/>
     <sheet name="MUV" sheetId="2" r:id="rId2"/>
     <sheet name="pritisak" sheetId="3" r:id="rId3"/>
     <sheet name="padavine" sheetId="4" r:id="rId4"/>
@@ -609,8 +609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O34" sqref="O34"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3500,7 +3500,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O1048576"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12310,7 +12310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -21819,7 +21819,7 @@
   <dimension ref="A1:O63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:O1048576"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>